<commit_message>
Adding Rule No Coma and Alert Upload
</commit_message>
<xml_diff>
--- a/public/files/Template_Sales_New.xlsx
+++ b/public/files/Template_Sales_New.xlsx
@@ -192,11 +192,11 @@
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,9 +213,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,19 +230,21 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,24 +265,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,25 +289,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -320,7 +305,23 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -343,7 +344,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,16 +356,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,187 +396,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,8 +748,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -778,6 +765,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -835,169 +842,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,15 +1001,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1030,12 +1017,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="176" fontId="0" fillId="6" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1362,7 +1349,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update Colomn and Templete (- Replace rule)
</commit_message>
<xml_diff>
--- a/public/files/Template_Sales_New.xlsx
+++ b/public/files/Template_Sales_New.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8300"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
@@ -839,7 +839,10 @@
   <dimension ref="A1:AF87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G9:G10"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -900,50 +903,50 @@
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="U1" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="V1" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="W1" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="X1" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z1" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB1" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC1" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD1" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE1" s="26" t="s">
-        <v>15</v>
       </c>
       <c r="AF1" s="27" t="s">
         <v>56</v>
@@ -974,68 +977,68 @@
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
       <c r="P2" s="20"/>
-      <c r="Q2" s="6">
-        <f>SUM(E2:J2)</f>
-        <v>0</v>
-      </c>
-      <c r="R2" s="6">
-        <f>SUM(K2:P2)</f>
-        <v>0</v>
-      </c>
-      <c r="S2" s="7">
-        <f>Q2+R2</f>
+      <c r="Q2" s="28">
+        <f>ROUND(E2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="28">
+        <f>ROUND(F2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="28">
+        <f>ROUND(G2,0)</f>
         <v>0</v>
       </c>
       <c r="T2" s="28">
-        <f>ROUND(E2,0)</f>
+        <f>ROUND(H2,0)</f>
         <v>0</v>
       </c>
       <c r="U2" s="28">
-        <f t="shared" ref="U2:AE2" si="0">ROUND(F2,0)</f>
+        <f>ROUND(I2,0)</f>
         <v>0</v>
       </c>
       <c r="V2" s="28">
-        <f t="shared" si="0"/>
+        <f>ROUND(J2,0)</f>
         <v>0</v>
       </c>
       <c r="W2" s="28">
-        <f t="shared" si="0"/>
+        <f>ROUND(K2,0)</f>
         <v>0</v>
       </c>
       <c r="X2" s="28">
-        <f t="shared" si="0"/>
+        <f>ROUND(L2,0)</f>
         <v>0</v>
       </c>
       <c r="Y2" s="28">
-        <f t="shared" si="0"/>
+        <f>ROUND(M2,0)</f>
         <v>0</v>
       </c>
       <c r="Z2" s="28">
-        <f t="shared" si="0"/>
+        <f>ROUND(N2,0)</f>
         <v>0</v>
       </c>
       <c r="AA2" s="28">
-        <f t="shared" si="0"/>
+        <f>ROUND(O2,0)</f>
         <v>0</v>
       </c>
       <c r="AB2" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC2" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD2" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE2" s="28">
-        <f t="shared" si="0"/>
+        <f>ROUND(P2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC2" s="6">
+        <f>SUM(Q2:V2)</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" s="6">
+        <f>SUM(W2:AB2)</f>
+        <v>0</v>
+      </c>
+      <c r="AE2" s="7">
+        <f>AC2+AD2</f>
         <v>0</v>
       </c>
       <c r="AF2" s="29">
-        <f>SUM(T2:AE2)-S2</f>
+        <f>SUM(Q2:AB2)-AE2</f>
         <v>0</v>
       </c>
     </row>
@@ -1064,68 +1067,68 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
-      <c r="Q3" s="6">
-        <f t="shared" ref="Q3:Q22" si="1">SUM(E3:J3)</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="6">
-        <f t="shared" ref="R3:R22" si="2">SUM(K3:P3)</f>
-        <v>0</v>
-      </c>
-      <c r="S3" s="7">
-        <f t="shared" ref="S3:S22" si="3">Q3+R3</f>
+      <c r="Q3" s="28">
+        <f t="shared" ref="Q3:Q22" si="0">ROUND(E3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="28">
+        <f t="shared" ref="R3:R22" si="1">ROUND(F3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="28">
+        <f t="shared" ref="S3:S22" si="2">ROUND(G3,0)</f>
         <v>0</v>
       </c>
       <c r="T3" s="28">
-        <f t="shared" ref="T3:T22" si="4">ROUND(E3,0)</f>
+        <f t="shared" ref="T3:T22" si="3">ROUND(H3,0)</f>
         <v>0</v>
       </c>
       <c r="U3" s="28">
-        <f t="shared" ref="U3:U22" si="5">ROUND(F3,0)</f>
+        <f t="shared" ref="U3:U22" si="4">ROUND(I3,0)</f>
         <v>0</v>
       </c>
       <c r="V3" s="28">
-        <f t="shared" ref="V3:V22" si="6">ROUND(G3,0)</f>
+        <f t="shared" ref="V3:V22" si="5">ROUND(J3,0)</f>
         <v>0</v>
       </c>
       <c r="W3" s="28">
-        <f t="shared" ref="W3:W22" si="7">ROUND(H3,0)</f>
+        <f t="shared" ref="W3:W22" si="6">ROUND(K3,0)</f>
         <v>0</v>
       </c>
       <c r="X3" s="28">
-        <f t="shared" ref="X3:X22" si="8">ROUND(I3,0)</f>
+        <f t="shared" ref="X3:X22" si="7">ROUND(L3,0)</f>
         <v>0</v>
       </c>
       <c r="Y3" s="28">
-        <f t="shared" ref="Y3:Y22" si="9">ROUND(J3,0)</f>
+        <f t="shared" ref="Y3:Y22" si="8">ROUND(M3,0)</f>
         <v>0</v>
       </c>
       <c r="Z3" s="28">
-        <f t="shared" ref="Z3:Z22" si="10">ROUND(K3,0)</f>
+        <f t="shared" ref="Z3:Z22" si="9">ROUND(N3,0)</f>
         <v>0</v>
       </c>
       <c r="AA3" s="28">
-        <f t="shared" ref="AA3:AA22" si="11">ROUND(L3,0)</f>
+        <f t="shared" ref="AA3:AA22" si="10">ROUND(O3,0)</f>
         <v>0</v>
       </c>
       <c r="AB3" s="28">
-        <f t="shared" ref="AB3:AB22" si="12">ROUND(M3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC3" s="28">
-        <f t="shared" ref="AC3:AC22" si="13">ROUND(N3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AD3" s="28">
-        <f t="shared" ref="AD3:AD22" si="14">ROUND(O3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE3" s="28">
-        <f t="shared" ref="AE3:AE22" si="15">ROUND(P3,0)</f>
+        <f t="shared" ref="AB3:AB22" si="11">ROUND(P3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="6">
+        <f t="shared" ref="AC3:AC22" si="12">SUM(Q3:V3)</f>
+        <v>0</v>
+      </c>
+      <c r="AD3" s="6">
+        <f t="shared" ref="AD3:AD22" si="13">SUM(W3:AB3)</f>
+        <v>0</v>
+      </c>
+      <c r="AE3" s="7">
+        <f t="shared" ref="AE3:AE22" si="14">AC3+AD3</f>
         <v>0</v>
       </c>
       <c r="AF3" s="29">
-        <f t="shared" ref="AF3:AF22" si="16">SUM(T3:AE3)-S3</f>
+        <f>SUM(Q3:AB3)-AE3</f>
         <v>0</v>
       </c>
     </row>
@@ -1154,68 +1157,68 @@
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
       <c r="P4" s="20"/>
-      <c r="Q4" s="6">
+      <c r="Q4" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R4" s="6">
+      <c r="S4" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S4" s="7">
+      <c r="T4" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T4" s="28">
+      <c r="U4" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U4" s="28">
+      <c r="V4" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V4" s="28">
+      <c r="W4" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W4" s="28">
+      <c r="X4" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X4" s="28">
+      <c r="Y4" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y4" s="28">
+      <c r="Z4" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z4" s="28">
+      <c r="AA4" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA4" s="28">
+      <c r="AB4" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB4" s="28">
+      <c r="AC4" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC4" s="28">
+      <c r="AD4" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD4" s="28">
+      <c r="AE4" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE4" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF4" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q4:AB4)-AE4</f>
         <v>0</v>
       </c>
     </row>
@@ -1244,68 +1247,68 @@
       <c r="N5" s="20"/>
       <c r="O5" s="20"/>
       <c r="P5" s="20"/>
-      <c r="Q5" s="6">
+      <c r="Q5" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R5" s="6">
+      <c r="S5" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S5" s="7">
+      <c r="T5" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T5" s="28">
+      <c r="U5" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U5" s="28">
+      <c r="V5" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V5" s="28">
+      <c r="W5" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W5" s="28">
+      <c r="X5" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X5" s="28">
+      <c r="Y5" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y5" s="28">
+      <c r="Z5" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z5" s="28">
+      <c r="AA5" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA5" s="28">
+      <c r="AB5" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB5" s="28">
+      <c r="AC5" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC5" s="28">
+      <c r="AD5" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD5" s="28">
+      <c r="AE5" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE5" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF5" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q5:AB5)-AE5</f>
         <v>0</v>
       </c>
     </row>
@@ -1334,68 +1337,68 @@
       <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="20"/>
-      <c r="Q6" s="6">
+      <c r="Q6" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R6" s="6">
+      <c r="S6" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S6" s="7">
+      <c r="T6" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T6" s="28">
+      <c r="U6" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U6" s="28">
+      <c r="V6" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V6" s="28">
+      <c r="W6" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W6" s="28">
+      <c r="X6" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X6" s="28">
+      <c r="Y6" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y6" s="28">
+      <c r="Z6" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z6" s="28">
+      <c r="AA6" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="28">
+      <c r="AB6" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="28">
+      <c r="AC6" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC6" s="28">
+      <c r="AD6" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="28">
+      <c r="AE6" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE6" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF6" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q6:AB6)-AE6</f>
         <v>0</v>
       </c>
     </row>
@@ -1424,68 +1427,68 @@
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
-      <c r="Q7" s="6">
+      <c r="Q7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R7" s="6">
+      <c r="S7" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S7" s="7">
+      <c r="T7" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T7" s="28">
+      <c r="U7" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U7" s="28">
+      <c r="V7" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V7" s="28">
+      <c r="W7" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W7" s="28">
+      <c r="X7" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X7" s="28">
+      <c r="Y7" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y7" s="28">
+      <c r="Z7" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z7" s="28">
+      <c r="AA7" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA7" s="28">
+      <c r="AB7" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB7" s="28">
+      <c r="AC7" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC7" s="28">
+      <c r="AD7" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="28">
+      <c r="AE7" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE7" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF7" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q7:AB7)-AE7</f>
         <v>0</v>
       </c>
     </row>
@@ -1514,68 +1517,68 @@
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
-      <c r="Q8" s="8">
+      <c r="Q8" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R8" s="8">
+      <c r="S8" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S8" s="9">
+      <c r="T8" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T8" s="28">
+      <c r="U8" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U8" s="28">
+      <c r="V8" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V8" s="28">
+      <c r="W8" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W8" s="28">
+      <c r="X8" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X8" s="28">
+      <c r="Y8" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y8" s="28">
+      <c r="Z8" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z8" s="28">
+      <c r="AA8" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA8" s="28">
+      <c r="AB8" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB8" s="28">
+      <c r="AC8" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC8" s="28">
+      <c r="AD8" s="8">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD8" s="28">
+      <c r="AE8" s="9">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE8" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF8" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q8:AB8)-AE8</f>
         <v>0</v>
       </c>
     </row>
@@ -1604,68 +1607,68 @@
       <c r="N9" s="23"/>
       <c r="O9" s="23"/>
       <c r="P9" s="23"/>
-      <c r="Q9" s="10">
+      <c r="Q9" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R9" s="10">
+      <c r="S9" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S9" s="11">
+      <c r="T9" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T9" s="28">
+      <c r="U9" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U9" s="28">
+      <c r="V9" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V9" s="28">
+      <c r="W9" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W9" s="28">
+      <c r="X9" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X9" s="28">
+      <c r="Y9" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y9" s="28">
+      <c r="Z9" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z9" s="28">
+      <c r="AA9" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA9" s="28">
+      <c r="AB9" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB9" s="28">
+      <c r="AC9" s="10">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC9" s="28">
+      <c r="AD9" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD9" s="28">
+      <c r="AE9" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE9" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF9" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q9:AB9)-AE9</f>
         <v>0</v>
       </c>
     </row>
@@ -1694,68 +1697,68 @@
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
-      <c r="Q10" s="6">
+      <c r="Q10" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R10" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R10" s="6">
+      <c r="S10" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S10" s="7">
+      <c r="T10" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T10" s="28">
+      <c r="U10" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U10" s="28">
+      <c r="V10" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V10" s="28">
+      <c r="W10" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W10" s="28">
+      <c r="X10" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X10" s="28">
+      <c r="Y10" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y10" s="28">
+      <c r="Z10" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z10" s="28">
+      <c r="AA10" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA10" s="28">
+      <c r="AB10" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB10" s="28">
+      <c r="AC10" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC10" s="28">
+      <c r="AD10" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD10" s="28">
+      <c r="AE10" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE10" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF10" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q10:AB10)-AE10</f>
         <v>0</v>
       </c>
     </row>
@@ -1784,68 +1787,68 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
       <c r="P11" s="23"/>
-      <c r="Q11" s="6">
+      <c r="Q11" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R11" s="6">
+      <c r="S11" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S11" s="7">
+      <c r="T11" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T11" s="28">
+      <c r="U11" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U11" s="28">
+      <c r="V11" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V11" s="28">
+      <c r="W11" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W11" s="28">
+      <c r="X11" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X11" s="28">
+      <c r="Y11" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y11" s="28">
+      <c r="Z11" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z11" s="28">
+      <c r="AA11" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA11" s="28">
+      <c r="AB11" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB11" s="28">
+      <c r="AC11" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC11" s="28">
+      <c r="AD11" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="28">
+      <c r="AE11" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE11" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF11" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q11:AB11)-AE11</f>
         <v>0</v>
       </c>
     </row>
@@ -1874,68 +1877,68 @@
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="6">
+      <c r="Q12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R12" s="6">
+      <c r="S12" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S12" s="7">
+      <c r="T12" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T12" s="28">
+      <c r="U12" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U12" s="28">
+      <c r="V12" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V12" s="28">
+      <c r="W12" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W12" s="28">
+      <c r="X12" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X12" s="28">
+      <c r="Y12" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y12" s="28">
+      <c r="Z12" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z12" s="28">
+      <c r="AA12" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA12" s="28">
+      <c r="AB12" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB12" s="28">
+      <c r="AC12" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC12" s="28">
+      <c r="AD12" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD12" s="28">
+      <c r="AE12" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE12" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF12" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q12:AB12)-AE12</f>
         <v>0</v>
       </c>
     </row>
@@ -1964,68 +1967,68 @@
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
       <c r="P13" s="23"/>
-      <c r="Q13" s="6">
+      <c r="Q13" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R13" s="6">
+      <c r="S13" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S13" s="7">
+      <c r="T13" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T13" s="28">
+      <c r="U13" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U13" s="28">
+      <c r="V13" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V13" s="28">
+      <c r="W13" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W13" s="28">
+      <c r="X13" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X13" s="28">
+      <c r="Y13" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y13" s="28">
+      <c r="Z13" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z13" s="28">
+      <c r="AA13" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA13" s="28">
+      <c r="AB13" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB13" s="28">
+      <c r="AC13" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC13" s="28">
+      <c r="AD13" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD13" s="28">
+      <c r="AE13" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE13" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF13" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q13:AB13)-AE13</f>
         <v>0</v>
       </c>
     </row>
@@ -2054,68 +2057,68 @@
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
-      <c r="Q14" s="6">
+      <c r="Q14" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R14" s="6">
+      <c r="S14" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S14" s="7">
+      <c r="T14" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T14" s="28">
+      <c r="U14" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U14" s="28">
+      <c r="V14" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V14" s="28">
+      <c r="W14" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W14" s="28">
+      <c r="X14" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X14" s="28">
+      <c r="Y14" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y14" s="28">
+      <c r="Z14" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z14" s="28">
+      <c r="AA14" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA14" s="28">
+      <c r="AB14" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB14" s="28">
+      <c r="AC14" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC14" s="28">
+      <c r="AD14" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD14" s="28">
+      <c r="AE14" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE14" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF14" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q14:AB14)-AE14</f>
         <v>0</v>
       </c>
     </row>
@@ -2144,68 +2147,68 @@
       <c r="N15" s="22"/>
       <c r="O15" s="22"/>
       <c r="P15" s="22"/>
-      <c r="Q15" s="8">
+      <c r="Q15" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R15" s="8">
+      <c r="S15" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S15" s="9">
+      <c r="T15" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T15" s="28">
+      <c r="U15" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U15" s="28">
+      <c r="V15" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V15" s="28">
+      <c r="W15" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W15" s="28">
+      <c r="X15" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X15" s="28">
+      <c r="Y15" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y15" s="28">
+      <c r="Z15" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z15" s="28">
+      <c r="AA15" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA15" s="28">
+      <c r="AB15" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB15" s="28">
+      <c r="AC15" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC15" s="28">
+      <c r="AD15" s="8">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD15" s="28">
+      <c r="AE15" s="9">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE15" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF15" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q15:AB15)-AE15</f>
         <v>0</v>
       </c>
     </row>
@@ -2234,68 +2237,68 @@
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23"/>
-      <c r="Q16" s="10">
+      <c r="Q16" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R16" s="10">
+      <c r="S16" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S16" s="11">
+      <c r="T16" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T16" s="28">
+      <c r="U16" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U16" s="28">
+      <c r="V16" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V16" s="28">
+      <c r="W16" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W16" s="28">
+      <c r="X16" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X16" s="28">
+      <c r="Y16" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y16" s="28">
+      <c r="Z16" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z16" s="28">
+      <c r="AA16" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA16" s="28">
+      <c r="AB16" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB16" s="28">
+      <c r="AC16" s="10">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC16" s="28">
+      <c r="AD16" s="10">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD16" s="28">
+      <c r="AE16" s="11">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE16" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF16" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q16:AB16)-AE16</f>
         <v>0</v>
       </c>
     </row>
@@ -2324,68 +2327,68 @@
       <c r="N17" s="23"/>
       <c r="O17" s="23"/>
       <c r="P17" s="23"/>
-      <c r="Q17" s="6">
+      <c r="Q17" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R17" s="6">
+      <c r="S17" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S17" s="7">
+      <c r="T17" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T17" s="28">
+      <c r="U17" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U17" s="28">
+      <c r="V17" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V17" s="28">
+      <c r="W17" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W17" s="28">
+      <c r="X17" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X17" s="28">
+      <c r="Y17" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y17" s="28">
+      <c r="Z17" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z17" s="28">
+      <c r="AA17" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA17" s="28">
+      <c r="AB17" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB17" s="28">
+      <c r="AC17" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC17" s="28">
+      <c r="AD17" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD17" s="28">
+      <c r="AE17" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE17" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF17" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q17:AB17)-AE17</f>
         <v>0</v>
       </c>
     </row>
@@ -2414,68 +2417,68 @@
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="23"/>
-      <c r="Q18" s="6">
+      <c r="Q18" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R18" s="6">
+      <c r="S18" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S18" s="7">
+      <c r="T18" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T18" s="28">
+      <c r="U18" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U18" s="28">
+      <c r="V18" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V18" s="28">
+      <c r="W18" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W18" s="28">
+      <c r="X18" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X18" s="28">
+      <c r="Y18" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y18" s="28">
+      <c r="Z18" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z18" s="28">
+      <c r="AA18" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA18" s="28">
+      <c r="AB18" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB18" s="28">
+      <c r="AC18" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC18" s="28">
+      <c r="AD18" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD18" s="28">
+      <c r="AE18" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE18" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF18" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q18:AB18)-AE18</f>
         <v>0</v>
       </c>
     </row>
@@ -2504,68 +2507,68 @@
       <c r="N19" s="23"/>
       <c r="O19" s="23"/>
       <c r="P19" s="23"/>
-      <c r="Q19" s="6">
+      <c r="Q19" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R19" s="6">
+      <c r="S19" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S19" s="7">
+      <c r="T19" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T19" s="28">
+      <c r="U19" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U19" s="28">
+      <c r="V19" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V19" s="28">
+      <c r="W19" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W19" s="28">
+      <c r="X19" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X19" s="28">
+      <c r="Y19" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y19" s="28">
+      <c r="Z19" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z19" s="28">
+      <c r="AA19" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA19" s="28">
+      <c r="AB19" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB19" s="28">
+      <c r="AC19" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC19" s="28">
+      <c r="AD19" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD19" s="28">
+      <c r="AE19" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE19" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF19" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q19:AB19)-AE19</f>
         <v>0</v>
       </c>
     </row>
@@ -2594,68 +2597,68 @@
       <c r="N20" s="23"/>
       <c r="O20" s="23"/>
       <c r="P20" s="23"/>
-      <c r="Q20" s="6">
+      <c r="Q20" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R20" s="6">
+      <c r="S20" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S20" s="7">
+      <c r="T20" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T20" s="28">
+      <c r="U20" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U20" s="28">
+      <c r="V20" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V20" s="28">
+      <c r="W20" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W20" s="28">
+      <c r="X20" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X20" s="28">
+      <c r="Y20" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y20" s="28">
+      <c r="Z20" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z20" s="28">
+      <c r="AA20" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA20" s="28">
+      <c r="AB20" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB20" s="28">
+      <c r="AC20" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC20" s="28">
+      <c r="AD20" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD20" s="28">
+      <c r="AE20" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE20" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF20" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q20:AB20)-AE20</f>
         <v>0</v>
       </c>
     </row>
@@ -2684,68 +2687,68 @@
       <c r="N21" s="23"/>
       <c r="O21" s="23"/>
       <c r="P21" s="23"/>
-      <c r="Q21" s="6">
+      <c r="Q21" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R21" s="6">
+      <c r="S21" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S21" s="7">
+      <c r="T21" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T21" s="28">
+      <c r="U21" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U21" s="28">
+      <c r="V21" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V21" s="28">
+      <c r="W21" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W21" s="28">
+      <c r="X21" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X21" s="28">
+      <c r="Y21" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y21" s="28">
+      <c r="Z21" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z21" s="28">
+      <c r="AA21" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA21" s="28">
+      <c r="AB21" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB21" s="28">
+      <c r="AC21" s="6">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC21" s="28">
+      <c r="AD21" s="6">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD21" s="28">
+      <c r="AE21" s="7">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE21" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF21" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q21:AB21)-AE21</f>
         <v>0</v>
       </c>
     </row>
@@ -2774,68 +2777,68 @@
       <c r="N22" s="22"/>
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
-      <c r="Q22" s="8">
+      <c r="Q22" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R22" s="8">
+      <c r="S22" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S22" s="9">
+      <c r="T22" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T22" s="28">
+      <c r="U22" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U22" s="28">
+      <c r="V22" s="28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V22" s="28">
+      <c r="W22" s="28">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W22" s="28">
+      <c r="X22" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X22" s="28">
+      <c r="Y22" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y22" s="28">
+      <c r="Z22" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z22" s="28">
+      <c r="AA22" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AA22" s="28">
+      <c r="AB22" s="28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB22" s="28">
+      <c r="AC22" s="8">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC22" s="28">
+      <c r="AD22" s="8">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AD22" s="28">
+      <c r="AE22" s="9">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AE22" s="28">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="AF22" s="29">
-        <f t="shared" si="16"/>
+        <f>SUM(Q22:AB22)-AE22</f>
         <v>0</v>
       </c>
     </row>
@@ -3750,10 +3753,10 @@
       <c r="P87" s="24"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MP7UejGsmcBS6gJkT9vruUVImX7/1S7aHsAu73ESoB/WHeALX109WFjVtOrLVieo0nBV2raO013Qqv6cFcW2Xg==" saltValue="PiWIDVBjewrTlMXpmB6zfw==" spinCount="100000" sheet="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="K0kHTlDbGVCYg+G4emEHVr0iXD2H1IvONf9ehvasWOTZE45FTbx4JyaTos8NMMInt+L2ssI+q5vhZsVSjDQNng==" saltValue="EKA7drCwxZ4z9hEMUQmTtQ==" spinCount="100000" sheet="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <protectedRanges>
     <protectedRange sqref="E1:P1048576" name="OPEN 1"/>
-    <protectedRange sqref="A23:XFD111" name="OPEN 2"/>
+    <protectedRange sqref="A23:P111 Q23:XFD111" name="OPEN 2"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Dev 1.1.0 : Update Templete
</commit_message>
<xml_diff>
--- a/public/files/Template_Sales_New.xlsx
+++ b/public/files/Template_Sales_New.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\#AIIA\2022\Trial SYSTEM BUDGET\Trial 15-11\New template 15-11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neli\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>ACC CODE</t>
   </si>
@@ -74,15 +74,6 @@
     <t>MAR</t>
   </si>
   <si>
-    <t>FY 2022 1st</t>
-  </si>
-  <si>
-    <t>FY 2022 2nd</t>
-  </si>
-  <si>
-    <t>FY 2022 TOTAL</t>
-  </si>
-  <si>
     <t>Sales (97%)</t>
   </si>
   <si>
@@ -194,19 +185,24 @@
     <t>SAL0036</t>
   </si>
   <si>
-    <t>Checking</t>
+    <t>FY 2023 1st</t>
+  </si>
+  <si>
+    <t>FY 2023 2nd</t>
+  </si>
+  <si>
+    <t>FY 2023 TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,22 +225,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,20 +269,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD8D8D8"/>
-        <bgColor rgb="FFD8D8D8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -469,36 +439,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -544,17 +490,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="3" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -836,13 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF87"/>
+  <dimension ref="A1:S87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC24" sqref="AC24"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -851,10 +783,11 @@
     <col min="2" max="2" width="15.36328125" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="32" width="20.08984375" customWidth="1"/>
+    <col min="5" max="16" width="14.26953125" customWidth="1"/>
+    <col min="17" max="19" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -903,67 +836,28 @@
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="X1" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y1" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z1" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA1" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB1" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF1" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="Q1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="13">
         <v>4111000101</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" s="20"/>
       <c r="F2" s="20"/>
@@ -977,83 +871,31 @@
       <c r="N2" s="20"/>
       <c r="O2" s="20"/>
       <c r="P2" s="20"/>
-      <c r="Q2" s="28">
-        <f>ROUND(E2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R2" s="28">
-        <f>ROUND(F2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="S2" s="28">
-        <f>ROUND(G2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="T2" s="28">
-        <f>ROUND(H2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U2" s="28">
-        <f>ROUND(I2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="V2" s="28">
-        <f>ROUND(J2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W2" s="28">
-        <f>ROUND(K2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="X2" s="28">
-        <f>ROUND(L2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y2" s="28">
-        <f>ROUND(M2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z2" s="28">
-        <f>ROUND(N2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA2" s="28">
-        <f>ROUND(O2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB2" s="28">
-        <f>ROUND(P2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC2" s="6">
-        <f>SUM(Q2:V2)</f>
-        <v>0</v>
-      </c>
-      <c r="AD2" s="6">
-        <f>SUM(W2:AB2)</f>
-        <v>0</v>
-      </c>
-      <c r="AE2" s="7">
-        <f>AC2+AD2</f>
-        <v>0</v>
-      </c>
-      <c r="AF2" s="29">
-        <f>SUM(Q2:AB2)-AE2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="Q2" s="6">
+        <f>SUM(E2:J2)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="6">
+        <f>SUM(K2:P2)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="7">
+        <f>Q2+R2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -1067,83 +909,31 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
-      <c r="Q3" s="28">
-        <f t="shared" ref="Q3:Q22" si="0">ROUND(E3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="28">
-        <f t="shared" ref="R3:R22" si="1">ROUND(F3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="S3" s="28">
-        <f t="shared" ref="S3:S22" si="2">ROUND(G3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="28">
-        <f t="shared" ref="T3:T22" si="3">ROUND(H3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U3" s="28">
-        <f t="shared" ref="U3:U22" si="4">ROUND(I3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="V3" s="28">
-        <f t="shared" ref="V3:V22" si="5">ROUND(J3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W3" s="28">
-        <f t="shared" ref="W3:W22" si="6">ROUND(K3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="X3" s="28">
-        <f t="shared" ref="X3:X22" si="7">ROUND(L3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y3" s="28">
-        <f t="shared" ref="Y3:Y22" si="8">ROUND(M3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z3" s="28">
-        <f t="shared" ref="Z3:Z22" si="9">ROUND(N3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA3" s="28">
-        <f t="shared" ref="AA3:AA22" si="10">ROUND(O3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="28">
-        <f t="shared" ref="AB3:AB22" si="11">ROUND(P3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC3" s="6">
-        <f t="shared" ref="AC3:AC22" si="12">SUM(Q3:V3)</f>
-        <v>0</v>
-      </c>
-      <c r="AD3" s="6">
-        <f t="shared" ref="AD3:AD22" si="13">SUM(W3:AB3)</f>
-        <v>0</v>
-      </c>
-      <c r="AE3" s="7">
-        <f t="shared" ref="AE3:AE22" si="14">AC3+AD3</f>
-        <v>0</v>
-      </c>
-      <c r="AF3" s="29">
-        <f>SUM(Q3:AB3)-AE3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="Q3" s="6">
+        <f t="shared" ref="Q3:Q22" si="0">SUM(E3:J3)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="6">
+        <f t="shared" ref="R3:R22" si="1">SUM(K3:P3)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="7">
+        <f t="shared" ref="S3:S22" si="2">Q3+R3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="20"/>
@@ -1157,83 +947,31 @@
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
       <c r="P4" s="20"/>
-      <c r="Q4" s="28">
+      <c r="Q4" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R4" s="28">
+      <c r="R4" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S4" s="28">
+      <c r="S4" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T4" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U4" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V4" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W4" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X4" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y4" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z4" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA4" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB4" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC4" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE4" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF4" s="29">
-        <f>SUM(Q4:AB4)-AE4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="20"/>
@@ -1247,83 +985,31 @@
       <c r="N5" s="20"/>
       <c r="O5" s="20"/>
       <c r="P5" s="20"/>
-      <c r="Q5" s="28">
+      <c r="Q5" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R5" s="28">
+      <c r="R5" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S5" s="28">
+      <c r="S5" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T5" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U5" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V5" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W5" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X5" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y5" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC5" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD5" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE5" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF5" s="29">
-        <f>SUM(Q5:AB5)-AE5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="20"/>
@@ -1337,83 +1023,31 @@
       <c r="N6" s="20"/>
       <c r="O6" s="20"/>
       <c r="P6" s="20"/>
-      <c r="Q6" s="28">
+      <c r="Q6" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R6" s="28">
+      <c r="R6" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S6" s="28">
+      <c r="S6" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T6" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U6" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V6" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W6" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X6" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y6" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA6" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC6" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD6" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE6" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF6" s="29">
-        <f>SUM(Q6:AB6)-AE6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
@@ -1427,83 +1061,31 @@
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
-      <c r="Q7" s="28">
+      <c r="Q7" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R7" s="28">
+      <c r="R7" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S7" s="28">
+      <c r="S7" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T7" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U7" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W7" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X7" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD7" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE7" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF7" s="29">
-        <f>SUM(Q7:AB7)-AE7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
@@ -1517,83 +1099,31 @@
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
-      <c r="Q8" s="28">
+      <c r="Q8" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R8" s="28">
+      <c r="R8" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S8" s="28">
+      <c r="S8" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T8" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U8" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V8" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X8" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y8" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC8" s="8">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD8" s="8">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE8" s="9">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF8" s="29">
-        <f>SUM(Q8:AB8)-AE8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="17">
         <v>4111000101</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
@@ -1607,83 +1137,31 @@
       <c r="N9" s="23"/>
       <c r="O9" s="23"/>
       <c r="P9" s="23"/>
-      <c r="Q9" s="28">
+      <c r="Q9" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R9" s="28">
+      <c r="R9" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S9" s="28">
+      <c r="S9" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T9" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U9" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V9" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W9" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X9" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y9" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z9" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC9" s="10">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD9" s="10">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE9" s="11">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF9" s="29">
-        <f>SUM(Q9:AB9)-AE9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
@@ -1697,83 +1175,31 @@
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
-      <c r="Q10" s="28">
+      <c r="Q10" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R10" s="28">
+      <c r="R10" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S10" s="28">
+      <c r="S10" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T10" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U10" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V10" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W10" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X10" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y10" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z10" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA10" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB10" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC10" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD10" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE10" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF10" s="29">
-        <f>SUM(Q10:AB10)-AE10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
@@ -1787,83 +1213,31 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
       <c r="P11" s="23"/>
-      <c r="Q11" s="28">
+      <c r="Q11" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R11" s="28">
+      <c r="R11" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S11" s="28">
+      <c r="S11" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T11" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U11" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V11" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W11" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X11" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y11" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z11" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA11" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB11" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC11" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD11" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE11" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF11" s="29">
-        <f>SUM(Q11:AB11)-AE11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="23"/>
@@ -1877,83 +1251,31 @@
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="28">
+      <c r="Q12" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R12" s="28">
+      <c r="R12" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S12" s="28">
+      <c r="S12" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T12" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U12" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V12" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W12" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X12" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y12" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z12" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA12" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC12" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD12" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE12" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF12" s="29">
-        <f>SUM(Q12:AB12)-AE12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
@@ -1967,83 +1289,31 @@
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
       <c r="P13" s="23"/>
-      <c r="Q13" s="28">
+      <c r="Q13" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R13" s="28">
+      <c r="R13" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S13" s="28">
+      <c r="S13" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T13" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U13" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V13" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W13" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X13" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y13" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z13" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA13" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC13" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD13" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE13" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF13" s="29">
-        <f>SUM(Q13:AB13)-AE13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
@@ -2057,83 +1327,31 @@
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
-      <c r="Q14" s="28">
+      <c r="Q14" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R14" s="28">
+      <c r="R14" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S14" s="28">
+      <c r="S14" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T14" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U14" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V14" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W14" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X14" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y14" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA14" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB14" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC14" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD14" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE14" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF14" s="29">
-        <f>SUM(Q14:AB14)-AE14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>40</v>
-      </c>
       <c r="D15" s="16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
@@ -2147,83 +1365,31 @@
       <c r="N15" s="22"/>
       <c r="O15" s="22"/>
       <c r="P15" s="22"/>
-      <c r="Q15" s="28">
+      <c r="Q15" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R15" s="28">
+      <c r="R15" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S15" s="28">
+      <c r="S15" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T15" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U15" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V15" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W15" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X15" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y15" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB15" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC15" s="8">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD15" s="8">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE15" s="9">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF15" s="29">
-        <f>SUM(Q15:AB15)-AE15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="17">
         <v>4111000101</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
@@ -2237,83 +1403,31 @@
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23"/>
-      <c r="Q16" s="28">
+      <c r="Q16" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S16" s="28">
+      <c r="S16" s="11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T16" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U16" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V16" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W16" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X16" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y16" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z16" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA16" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB16" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC16" s="10">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD16" s="10">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE16" s="11">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF16" s="29">
-        <f>SUM(Q16:AB16)-AE16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
@@ -2327,83 +1441,31 @@
       <c r="N17" s="23"/>
       <c r="O17" s="23"/>
       <c r="P17" s="23"/>
-      <c r="Q17" s="28">
+      <c r="Q17" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R17" s="28">
+      <c r="R17" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S17" s="28">
+      <c r="S17" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T17" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U17" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V17" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W17" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X17" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y17" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z17" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA17" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC17" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD17" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE17" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF17" s="29">
-        <f>SUM(Q17:AB17)-AE17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -2417,83 +1479,31 @@
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="23"/>
-      <c r="Q18" s="28">
+      <c r="Q18" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R18" s="28">
+      <c r="R18" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S18" s="28">
+      <c r="S18" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T18" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U18" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V18" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W18" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X18" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y18" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z18" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA18" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB18" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC18" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD18" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE18" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF18" s="29">
-        <f>SUM(Q18:AB18)-AE18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -2507,83 +1517,31 @@
       <c r="N19" s="23"/>
       <c r="O19" s="23"/>
       <c r="P19" s="23"/>
-      <c r="Q19" s="28">
+      <c r="Q19" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R19" s="28">
+      <c r="R19" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S19" s="28">
+      <c r="S19" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T19" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U19" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V19" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W19" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X19" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y19" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z19" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA19" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB19" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC19" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD19" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE19" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF19" s="29">
-        <f>SUM(Q19:AB19)-AE19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -2597,83 +1555,31 @@
       <c r="N20" s="23"/>
       <c r="O20" s="23"/>
       <c r="P20" s="23"/>
-      <c r="Q20" s="28">
+      <c r="Q20" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R20" s="28">
+      <c r="R20" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S20" s="28">
+      <c r="S20" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T20" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U20" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V20" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W20" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X20" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y20" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z20" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA20" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB20" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC20" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD20" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE20" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF20" s="29">
-        <f>SUM(Q20:AB20)-AE20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -2687,83 +1593,31 @@
       <c r="N21" s="23"/>
       <c r="O21" s="23"/>
       <c r="P21" s="23"/>
-      <c r="Q21" s="28">
+      <c r="Q21" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R21" s="28">
+      <c r="R21" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S21" s="28">
+      <c r="S21" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T21" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U21" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V21" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W21" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X21" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y21" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z21" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA21" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB21" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC21" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD21" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE21" s="7">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF21" s="29">
-        <f>SUM(Q21:AB21)-AE21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
@@ -2777,72 +1631,20 @@
       <c r="N22" s="22"/>
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
-      <c r="Q22" s="28">
+      <c r="Q22" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R22" s="28">
+      <c r="R22" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S22" s="28">
+      <c r="S22" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T22" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U22" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V22" s="28">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W22" s="28">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X22" s="28">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y22" s="28">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z22" s="28">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA22" s="28">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB22" s="28">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC22" s="8">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD22" s="8">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE22" s="9">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AF22" s="29">
-        <f>SUM(Q22:AB22)-AE22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24"/>
@@ -2856,7 +1658,7 @@
       <c r="O23" s="24"/>
       <c r="P23" s="24"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="24"/>
@@ -2870,7 +1672,7 @@
       <c r="O24" s="24"/>
       <c r="P24" s="24"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="24"/>
@@ -2884,7 +1686,7 @@
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="24"/>
@@ -2898,7 +1700,7 @@
       <c r="O26" s="24"/>
       <c r="P26" s="24"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
@@ -2912,7 +1714,7 @@
       <c r="O27" s="24"/>
       <c r="P27" s="24"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
       <c r="G28" s="24"/>
@@ -2926,7 +1728,7 @@
       <c r="O28" s="24"/>
       <c r="P28" s="24"/>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
       <c r="G29" s="24"/>
@@ -2940,7 +1742,7 @@
       <c r="O29" s="24"/>
       <c r="P29" s="24"/>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="24"/>
@@ -2954,7 +1756,7 @@
       <c r="O30" s="24"/>
       <c r="P30" s="24"/>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
@@ -2968,7 +1770,7 @@
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
       <c r="G32" s="24"/>
@@ -3753,10 +2555,10 @@
       <c r="P87" s="24"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="K0kHTlDbGVCYg+G4emEHVr0iXD2H1IvONf9ehvasWOTZE45FTbx4JyaTos8NMMInt+L2ssI+q5vhZsVSjDQNng==" saltValue="EKA7drCwxZ4z9hEMUQmTtQ==" spinCount="100000" sheet="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <protectedRanges>
+    <protectedRange sqref="A23:XFD111" name="OPEN 2"/>
     <protectedRange sqref="E1:P1048576" name="OPEN 1"/>
-    <protectedRange sqref="A23:P111 Q23:XFD111" name="OPEN 2"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>